<commit_message>
add 1 and 2 slides
</commit_message>
<xml_diff>
--- a/upn-surabaya/material/14_miniProjects/upn_surabaya.xlsx
+++ b/upn-surabaya/material/14_miniProjects/upn_surabaya.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mymac/Desktop/eppo/belajaR/upn-surabaya/14_miniProjects/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ujangfahmi/Desktop/Ujang Fahmi/Modul Sadasa/belajaR/upn-surabaya/material/14_miniProjects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD5FB7D-2B23-6C44-BC1A-D88466C0E9EC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D83D16C4-CB77-2946-BC4A-41DB67C4F123}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14260" xr2:uid="{80EF1E67-8656-5344-80C6-0662AE50915F}"/>
+    <workbookView xWindow="-37160" yWindow="-2260" windowWidth="25440" windowHeight="14260" xr2:uid="{80EF1E67-8656-5344-80C6-0662AE50915F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -79,7 +79,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -430,16 +430,16 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -447,7 +447,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17">
+    <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -455,7 +455,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="17">
+    <row r="3" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -463,7 +463,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -471,7 +471,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -479,7 +479,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -487,7 +487,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -495,7 +495,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -503,7 +503,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -511,7 +511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -519,7 +519,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -527,7 +527,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -535,7 +535,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -543,7 +543,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -551,7 +551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
add script material 2
</commit_message>
<xml_diff>
--- a/upn-surabaya/material/14_miniProjects/upn_surabaya.xlsx
+++ b/upn-surabaya/material/14_miniProjects/upn_surabaya.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ujangfahmi/Desktop/Ujang Fahmi/Modul Sadasa/belajaR/upn-surabaya/material/14_miniProjects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D83D16C4-CB77-2946-BC4A-41DB67C4F123}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7621F15-04A8-134D-92EE-ABB22C3A0FCA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-37160" yWindow="-2260" windowWidth="25440" windowHeight="14260" xr2:uid="{80EF1E67-8656-5344-80C6-0662AE50915F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
   <si>
     <t>Pengenalan Data Science dan R</t>
   </si>
@@ -72,7 +72,22 @@
     <t>material</t>
   </si>
   <si>
-    <t>hours</t>
+    <t>tanggal</t>
+  </si>
+  <si>
+    <t>jam</t>
+  </si>
+  <si>
+    <t>minggu</t>
+  </si>
+  <si>
+    <t>sept</t>
+  </si>
+  <si>
+    <t>oct</t>
+  </si>
+  <si>
+    <t>month</t>
   </si>
 </sst>
 </file>
@@ -88,15 +103,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -104,14 +125,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -427,139 +484,265 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6390157-31DB-644B-8849-6DEF8BA767EF}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="E1" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="B2" s="8">
+        <v>3</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="6">
+        <v>17</v>
+      </c>
+      <c r="E2" s="7">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    </row>
+    <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="8">
+        <v>3</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="6">
+        <v>18</v>
+      </c>
+      <c r="E3" s="7"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="B4" s="8">
+        <v>3</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="6">
+        <v>19</v>
+      </c>
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="2">
+        <v>24</v>
+      </c>
+      <c r="E5" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="B6" s="3">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="2">
+        <v>25</v>
+      </c>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="B7" s="3">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="2">
+        <v>26</v>
+      </c>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="B8" s="8">
+        <v>3</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="6">
+        <v>1</v>
+      </c>
+      <c r="E8" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="C9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="6">
+        <v>2</v>
+      </c>
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="C10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="6">
+        <v>2</v>
+      </c>
+      <c r="E10" s="7"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="B11" s="8">
+        <v>3</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="6">
+        <v>3</v>
+      </c>
+      <c r="E11" s="7"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="B12" s="3">
+        <v>3</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="2">
+        <v>8</v>
+      </c>
+      <c r="E12" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="C13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="2">
+        <v>9</v>
+      </c>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="C14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="2">
+        <v>10</v>
+      </c>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="8">
         <v>2</v>
       </c>
+      <c r="C15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="6">
+        <v>16</v>
+      </c>
+      <c r="E15" s="8">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="E12:E14"/>
+    <mergeCell ref="E8:E11"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="E2:E4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
hari ke 3 minggu 2
</commit_message>
<xml_diff>
--- a/upn-surabaya/material/14_miniProjects/upn_surabaya.xlsx
+++ b/upn-surabaya/material/14_miniProjects/upn_surabaya.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ujangfahmi/Desktop/Ujang Fahmi/Modul Sadasa/belajaR/upn-surabaya/material/14_miniProjects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7621F15-04A8-134D-92EE-ABB22C3A0FCA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37C3CE04-730B-6F46-8818-FF0B4E06EBCB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37160" yWindow="-2260" windowWidth="25440" windowHeight="14260" xr2:uid="{80EF1E67-8656-5344-80C6-0662AE50915F}"/>
+    <workbookView xWindow="25560" yWindow="-5140" windowWidth="38440" windowHeight="21140" xr2:uid="{80EF1E67-8656-5344-80C6-0662AE50915F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -117,7 +117,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -140,11 +140,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -155,9 +192,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -167,7 +201,34 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -487,7 +548,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -517,51 +578,51 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8">
-        <v>3</v>
-      </c>
-      <c r="C2" s="6" t="s">
+      <c r="B2" s="6">
+        <v>3</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="5">
         <v>17</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="8">
-        <v>3</v>
-      </c>
-      <c r="C3" s="6" t="s">
+      <c r="B3" s="6">
+        <v>3</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>18</v>
       </c>
-      <c r="E3" s="7"/>
+      <c r="E3" s="10"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="8">
-        <v>3</v>
-      </c>
-      <c r="C4" s="6" t="s">
+      <c r="B4" s="6">
+        <v>3</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>19</v>
       </c>
-      <c r="E4" s="7"/>
+      <c r="E4" s="10"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
@@ -576,7 +637,7 @@
       <c r="D5" s="2">
         <v>24</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="9">
         <v>2</v>
       </c>
     </row>
@@ -593,7 +654,7 @@
       <c r="D6" s="2">
         <v>25</v>
       </c>
-      <c r="E6" s="4"/>
+      <c r="E6" s="9"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
@@ -608,75 +669,75 @@
       <c r="D7" s="2">
         <v>26</v>
       </c>
-      <c r="E7" s="4"/>
+      <c r="E7" s="9"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="8">
         <v>3</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <v>1</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="11">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="8">
         <v>1</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <v>2</v>
       </c>
-      <c r="E9" s="7"/>
+      <c r="E9" s="12"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="8">
         <v>2</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="5">
         <v>2</v>
       </c>
-      <c r="E10" s="7"/>
+      <c r="E10" s="12"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="8">
         <v>3</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="6">
-        <v>3</v>
-      </c>
-      <c r="E11" s="7"/>
+      <c r="D11" s="5">
+        <v>3</v>
+      </c>
+      <c r="E11" s="13"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="7">
         <v>3</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -685,7 +746,7 @@
       <c r="D12" s="2">
         <v>8</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="14">
         <v>4</v>
       </c>
     </row>
@@ -693,7 +754,7 @@
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="7">
         <v>2</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -702,13 +763,13 @@
       <c r="D13" s="2">
         <v>9</v>
       </c>
-      <c r="E13" s="4"/>
+      <c r="E13" s="15"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="7">
         <v>1</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -717,19 +778,19 @@
       <c r="D14" s="2">
         <v>10</v>
       </c>
-      <c r="E14" s="4"/>
+      <c r="E14" s="16"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="8">
         <v>2</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="5">
         <v>16</v>
       </c>
       <c r="E15" s="8">

</xml_diff>

<commit_message>
add slide twitter api
</commit_message>
<xml_diff>
--- a/upn-surabaya/material/14_miniProjects/upn_surabaya.xlsx
+++ b/upn-surabaya/material/14_miniProjects/upn_surabaya.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ujangfahmi/Desktop/Ujang Fahmi/Modul Sadasa/belajaR/upn-surabaya/material/14_miniProjects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37C3CE04-730B-6F46-8818-FF0B4E06EBCB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CD92679-F670-8644-98DC-0AD29BAB122A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25560" yWindow="-5140" windowWidth="38440" windowHeight="21140" xr2:uid="{80EF1E67-8656-5344-80C6-0662AE50915F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="17120" windowHeight="14380" xr2:uid="{80EF1E67-8656-5344-80C6-0662AE50915F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="21">
   <si>
     <t>Pengenalan Data Science dan R</t>
   </si>
@@ -75,9 +75,6 @@
     <t>tanggal</t>
   </si>
   <si>
-    <t>jam</t>
-  </si>
-  <si>
     <t>minggu</t>
   </si>
   <si>
@@ -88,13 +85,16 @@
   </si>
   <si>
     <t>month</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -102,8 +102,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -112,12 +118,42 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -161,6 +197,19 @@
         <color indexed="64"/>
       </right>
       <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -168,6 +217,41 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -175,13 +259,24 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -189,53 +284,230 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="10">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -246,6 +518,20 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F74EA495-01F8-1A43-9208-F69A3D13D9F5}" name="Table1" displayName="Table1" ref="A1:E18" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" headerRowBorderDxfId="6" tableBorderDxfId="7" totalsRowBorderDxfId="5">
+  <autoFilter ref="A1:E18" xr:uid="{4377A1FF-BA14-6D40-A080-E5C454652446}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{C4610543-F372-CB4B-80C5-8960DE9A52FB}" name="No" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{F2803ACC-AB73-BD48-B2F1-42B7224DD82C}" name="material" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{9041FDD0-2F58-7D42-B540-188A8AFB4162}" name="month" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{5979FBC6-83CA-EF42-9B8F-7A2100FADF56}" name="tanggal" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{06C4264F-7CA1-3347-B950-B0E7D2E087B2}" name="minggu" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -545,265 +831,360 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6390157-31DB-644B-8849-6DEF8BA767EF}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.83203125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="9">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="D2" s="2">
+        <v>17</v>
+      </c>
+      <c r="E2" s="6">
+        <v>1</v>
+      </c>
+      <c r="F2" s="14"/>
+      <c r="G2" s="19"/>
+    </row>
+    <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="9"/>
+      <c r="B3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6">
-        <v>3</v>
-      </c>
-      <c r="C2" s="5" t="s">
+      <c r="C3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="2">
         <v>18</v>
       </c>
-      <c r="D2" s="5">
+      <c r="E3" s="6">
+        <v>1</v>
+      </c>
+      <c r="F3" s="14">
+        <v>1</v>
+      </c>
+      <c r="G3" s="19"/>
+    </row>
+    <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="9"/>
+      <c r="B4" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="10">
+      <c r="D4" s="2">
+        <v>19</v>
+      </c>
+      <c r="E4" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="F4" s="14"/>
+      <c r="G4" s="19"/>
+    </row>
+    <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="9">
+        <v>2</v>
+      </c>
+      <c r="B5" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="6">
-        <v>3</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="5">
-        <v>18</v>
-      </c>
-      <c r="E3" s="10"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="6">
-        <v>3</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="5">
-        <v>19</v>
-      </c>
-      <c r="E4" s="10"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="3">
-        <v>3</v>
-      </c>
       <c r="C5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" s="2">
         <v>24</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="3">
-        <v>3</v>
+      <c r="F5" s="15"/>
+      <c r="G5" s="19"/>
+    </row>
+    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="9"/>
+      <c r="B6" s="10" t="s">
+        <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="2">
         <v>25</v>
       </c>
-      <c r="E6" s="9"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="3">
-        <v>3</v>
+      <c r="E6" s="6">
+        <v>2</v>
+      </c>
+      <c r="F6" s="15">
+        <v>2</v>
+      </c>
+      <c r="G6" s="19"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="9">
+        <v>3</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" s="2">
         <v>26</v>
       </c>
-      <c r="E7" s="9"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
+      <c r="E7" s="6">
+        <v>2</v>
+      </c>
+      <c r="F7" s="15"/>
+      <c r="G7" s="19"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="9">
+        <v>1</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1</v>
+      </c>
+      <c r="E8" s="13">
+        <v>3</v>
+      </c>
+      <c r="F8" s="16"/>
+      <c r="G8" s="19"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="9">
+        <v>2</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="2">
+        <v>2</v>
+      </c>
+      <c r="E9" s="13">
+        <v>3</v>
+      </c>
+      <c r="F9" s="16"/>
+      <c r="G9" s="19"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="9">
+        <v>3</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="2">
+        <v>2</v>
+      </c>
+      <c r="E10" s="13">
+        <v>3</v>
+      </c>
+      <c r="F10" s="16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="9">
+        <v>4</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="2">
+        <v>3</v>
+      </c>
+      <c r="E11" s="13">
+        <v>3</v>
+      </c>
+      <c r="F11" s="16"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="9">
+        <v>5</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="2">
+        <v>3</v>
+      </c>
+      <c r="E12" s="13">
+        <v>3</v>
+      </c>
+      <c r="F12" s="16"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="9">
         <v>6</v>
       </c>
-      <c r="B8" s="8">
-        <v>3</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="5">
+      <c r="B13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="2">
+        <v>3</v>
+      </c>
+      <c r="E13" s="13">
+        <v>3</v>
+      </c>
+      <c r="F13" s="16"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="9">
         <v>1</v>
       </c>
-      <c r="E8" s="11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="8">
+      <c r="B14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="2">
+        <v>8</v>
+      </c>
+      <c r="E14" s="6">
+        <v>4</v>
+      </c>
+      <c r="F14" s="17"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="9">
+        <v>2</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="2">
+        <v>9</v>
+      </c>
+      <c r="E15" s="6">
+        <v>4</v>
+      </c>
+      <c r="F15" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="9">
+        <v>3</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="2">
+        <v>10</v>
+      </c>
+      <c r="E16" s="6">
+        <v>4</v>
+      </c>
+      <c r="F16" s="17"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="9">
+        <v>4</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="2">
+        <v>10</v>
+      </c>
+      <c r="E17" s="6">
+        <v>4</v>
+      </c>
+      <c r="F17" s="17"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="11">
         <v>1</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="5">
-        <v>2</v>
-      </c>
-      <c r="E9" s="12"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="8">
-        <v>2</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="5">
-        <v>2</v>
-      </c>
-      <c r="E10" s="12"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="8">
-        <v>3</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="5">
-        <v>3</v>
-      </c>
-      <c r="E11" s="13"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="7">
-        <v>3</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="2">
-        <v>8</v>
-      </c>
-      <c r="E12" s="14">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="7">
-        <v>2</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="2">
-        <v>9</v>
-      </c>
-      <c r="E13" s="15"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="7">
-        <v>1</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="2">
-        <v>10</v>
-      </c>
-      <c r="E14" s="16"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
+      <c r="B18" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="8">
-        <v>2</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="5">
+      <c r="C18" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="3">
         <v>16</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E18" s="12">
         <v>5</v>
       </c>
+      <c r="F18" s="18">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="E12:E14"/>
-    <mergeCell ref="E8:E11"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="E2:E4"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add slides sentiment and topic modeling
</commit_message>
<xml_diff>
--- a/upn-surabaya/material/14_miniProjects/upn_surabaya.xlsx
+++ b/upn-surabaya/material/14_miniProjects/upn_surabaya.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ujangfahmi/Desktop/Ujang Fahmi/Modul Sadasa/belajaR/upn-surabaya/material/14_miniProjects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CD92679-F670-8644-98DC-0AD29BAB122A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6019C5E-7E8F-FF48-974F-F3E6975F4869}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="17120" windowHeight="14380" xr2:uid="{80EF1E67-8656-5344-80C6-0662AE50915F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14380" xr2:uid="{80EF1E67-8656-5344-80C6-0662AE50915F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="22">
   <si>
     <t>Pengenalan Data Science dan R</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>Materi ke-</t>
   </si>
 </sst>
 </file>
@@ -276,7 +279,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -333,6 +336,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -458,13 +462,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -487,6 +484,13 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <fill>
@@ -521,7 +525,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F74EA495-01F8-1A43-9208-F69A3D13D9F5}" name="Table1" displayName="Table1" ref="A1:E18" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" headerRowBorderDxfId="6" tableBorderDxfId="7" totalsRowBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F74EA495-01F8-1A43-9208-F69A3D13D9F5}" name="Table1" displayName="Table1" ref="A1:E18" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6" totalsRowBorderDxfId="5">
   <autoFilter ref="A1:E18" xr:uid="{4377A1FF-BA14-6D40-A080-E5C454652446}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{C4610543-F372-CB4B-80C5-8960DE9A52FB}" name="No" dataDxfId="4"/>
@@ -834,7 +838,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -844,6 +848,7 @@
     <col min="3" max="3" width="8.83203125" customWidth="1"/>
     <col min="4" max="4" width="9.6640625" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" style="1"/>
+    <col min="7" max="7" width="10.83203125" style="20"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -862,6 +867,10 @@
       <c r="E1" s="8" t="s">
         <v>16</v>
       </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="19"/>
     </row>
     <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="9">
@@ -992,7 +1001,6 @@
         <v>3</v>
       </c>
       <c r="F8" s="16"/>
-      <c r="G8" s="19"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="9">
@@ -1011,7 +1019,6 @@
         <v>3</v>
       </c>
       <c r="F9" s="16"/>
-      <c r="G9" s="19"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="9">
@@ -1071,46 +1078,46 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="9">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D13" s="2">
-        <v>3</v>
-      </c>
-      <c r="E13" s="13">
-        <v>3</v>
-      </c>
-      <c r="F13" s="16"/>
+        <v>8</v>
+      </c>
+      <c r="E13" s="6">
+        <v>4</v>
+      </c>
+      <c r="F13" s="17"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D14" s="2">
-        <v>8</v>
-      </c>
-      <c r="E14" s="6">
+        <v>9</v>
+      </c>
+      <c r="E14" s="13">
         <v>4</v>
       </c>
       <c r="F14" s="17"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>18</v>
@@ -1127,7 +1134,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>11</v>
@@ -1145,7 +1152,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
update slide api twitter
</commit_message>
<xml_diff>
--- a/upn-surabaya/material/14_miniProjects/upn_surabaya.xlsx
+++ b/upn-surabaya/material/14_miniProjects/upn_surabaya.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ujangfahmi/Desktop/Ujang Fahmi/Modul Sadasa/belajaR/upn-surabaya/material/14_miniProjects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9375167-B785-7647-A5A0-DDB39C9F9B13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1863646-159A-7B49-B9FE-AABFA3915B07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25600" yWindow="-5140" windowWidth="38400" windowHeight="21140" xr2:uid="{80EF1E67-8656-5344-80C6-0662AE50915F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
   <si>
     <t>Pengenalan Data Science dan R</t>
   </si>
@@ -91,6 +91,12 @@
   </si>
   <si>
     <t>hari ke-</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>td</t>
   </si>
 </sst>
 </file>
@@ -850,7 +856,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -860,7 +866,7 @@
     <col min="3" max="3" width="8.83203125" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" style="1"/>
-    <col min="7" max="7" width="10.83203125" style="14"/>
+    <col min="7" max="7" width="6.5" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -1013,6 +1019,9 @@
         <v>3</v>
       </c>
       <c r="F8" s="12"/>
+      <c r="G8" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="15">
@@ -1031,6 +1040,9 @@
         <v>3</v>
       </c>
       <c r="F9" s="12"/>
+      <c r="G9" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="15">
@@ -1050,6 +1062,9 @@
       </c>
       <c r="F10" s="12">
         <v>3</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>